<commit_message>
feat: add template loader with template import and validation fix: constants.py
</commit_message>
<xml_diff>
--- a/sample/data/sample_non_retail.xlsx
+++ b/sample/data/sample_non_retail.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nexialog365-my.sharepoint.com/personal/hcle_nexialog_com/Documents/Documents/IFRS9-Simulation/sample/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="8_{61285AE1-AC17-415D-A2E0-C76875B0539E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CE478AB-30C1-4B30-AB0E-30041D057EF7}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="8_{61285AE1-AC17-415D-A2E0-C76875B0539E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBB27DF1-D772-4FD8-BC54-139D3AFD8078}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1897D71D-1AE5-42B2-8FF2-FE784E06C521}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
   <si>
     <t>Obligor_RCT</t>
   </si>
@@ -197,14 +197,26 @@
     <t>CCF</t>
   </si>
   <si>
-    <t>I-FINE</t>
+    <t>ABC200</t>
+  </si>
+  <si>
+    <t>100000002202024</t>
+  </si>
+  <si>
+    <t>789000002202024 X</t>
+  </si>
+  <si>
+    <t>LGD_value</t>
+  </si>
+  <si>
+    <t>I_FINE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,6 +228,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -241,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -250,6 +268,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,25 +606,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A264F5-EA5A-4E89-9EE3-75A8C0234AA0}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.453125" customWidth="1"/>
-    <col min="13" max="14" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -662,28 +683,31 @@
         <v>18</v>
       </c>
       <c r="T1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -699,7 +723,7 @@
       <c r="E2" t="s">
         <v>24</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="5">
         <v>6</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -741,29 +765,32 @@
       <c r="S2" t="s">
         <v>33</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2">
+        <v>0.35</v>
+      </c>
+      <c r="U2" t="s">
         <v>34</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>77011.53</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>35</v>
       </c>
-      <c r="W2" s="3">
+      <c r="X2" s="3">
         <v>45838</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>37</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>110</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -813,29 +840,32 @@
       <c r="S3" t="s">
         <v>32</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3">
+        <v>0.4</v>
+      </c>
+      <c r="U3" t="s">
         <v>34</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>30675</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>39</v>
       </c>
-      <c r="W3" s="3">
+      <c r="X3" s="3">
         <v>45838</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>37</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>176</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -885,26 +915,29 @@
       <c r="S4" t="s">
         <v>32</v>
       </c>
-      <c r="U4">
+      <c r="T4">
+        <v>0.4</v>
+      </c>
+      <c r="V4">
         <v>30675</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>39</v>
       </c>
-      <c r="W4" s="3">
+      <c r="X4" s="3">
         <v>45838</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>37</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>176</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -960,29 +993,104 @@
       <c r="S5" t="s">
         <v>32</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5">
+        <v>0.4</v>
+      </c>
+      <c r="U5" t="s">
+        <v>57</v>
+      </c>
+      <c r="V5">
+        <v>30675</v>
+      </c>
+      <c r="W5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X5" s="3">
+        <v>45838</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z5">
+        <v>176</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>53</v>
       </c>
-      <c r="U5">
-        <v>30675</v>
-      </c>
-      <c r="V5" t="s">
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" s="3">
+        <v>45808</v>
+      </c>
+      <c r="N6" s="3">
+        <v>45810</v>
+      </c>
+      <c r="P6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>31</v>
+      </c>
+      <c r="T6">
+        <v>0.45</v>
+      </c>
+      <c r="U6" t="s">
+        <v>57</v>
+      </c>
+      <c r="V6">
+        <v>138</v>
+      </c>
+      <c r="W6" t="s">
         <v>35</v>
       </c>
-      <c r="W5" s="3">
-        <v>45838</v>
-      </c>
-      <c r="X5" t="s">
+      <c r="X6" s="3">
+        <v>45808</v>
+      </c>
+      <c r="Y6" t="s">
         <v>37</v>
       </c>
-      <c r="Y5">
+      <c r="Z6">
         <v>176</v>
       </c>
-      <c r="Z5">
-        <v>1</v>
+      <c r="AA6">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add: param columns extension, interpolation, ead calculation
</commit_message>
<xml_diff>
--- a/sample/data/sample_non_retail.xlsx
+++ b/sample/data/sample_non_retail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nexialog365-my.sharepoint.com/personal/hcle_nexialog_com/Documents/Documents/IFRS9-Simulation/sample/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="8_{61285AE1-AC17-415D-A2E0-C76875B0539E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBB27DF1-D772-4FD8-BC54-139D3AFD8078}"/>
+  <xr:revisionPtr revIDLastSave="199" documentId="8_{61285AE1-AC17-415D-A2E0-C76875B0539E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22A6B18C-1474-40C7-9D0C-B008BA18D47F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1897D71D-1AE5-42B2-8FF2-FE784E06C521}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="61">
   <si>
     <t>Obligor_RCT</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>I_FINE</t>
+  </si>
+  <si>
+    <t>ABC300</t>
+  </si>
+  <si>
+    <t>100000002202025</t>
+  </si>
+  <si>
+    <t>789000002202025 X</t>
   </si>
 </sst>
 </file>
@@ -606,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A264F5-EA5A-4E89-9EE3-75A8C0234AA0}">
-  <dimension ref="A1:AA6"/>
+  <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1089,6 +1098,80 @@
         <v>0.4</v>
       </c>
     </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="3">
+        <v>45808</v>
+      </c>
+      <c r="N7" s="3">
+        <v>57881</v>
+      </c>
+      <c r="O7">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="P7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>31</v>
+      </c>
+      <c r="T7">
+        <v>0.45</v>
+      </c>
+      <c r="U7" t="s">
+        <v>34</v>
+      </c>
+      <c r="V7">
+        <v>1799989</v>
+      </c>
+      <c r="W7" t="s">
+        <v>35</v>
+      </c>
+      <c r="X7" s="3">
+        <v>45808</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z7">
+        <v>176</v>
+      </c>
+      <c r="AA7">
+        <v>0.4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>